<commit_message>
Vue Programm + AdobeXD pdf
</commit_message>
<xml_diff>
--- a/98-Arbeitsstunden/Arbeitsstunden_Lidauer.xlsx
+++ b/98-Arbeitsstunden/Arbeitsstunden_Lidauer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MANUEL\SCHOOL\GitHub\proproduction\98-Arbeitsstunden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3106003-A396-4C8B-967F-AB3B07166740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCD8B98-57A3-4785-BB4A-E2BF61C35833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Dokumente zusammengesucht + genauere Funktionen überlegt</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Vue Projekt getestet</t>
+  </si>
+  <si>
+    <t>AdobeXD GUI Modell fertig gestellt + Vue Navigation Bar informiert</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
       </c>
       <c r="H1" s="7">
         <f>SUM(E4:E88)</f>
-        <v>22.833333333333343</v>
+        <v>23.500000000000014</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>9</v>
@@ -855,9 +858,21 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43752</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.88194444444444453</v>
+      </c>
       <c r="E23" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.66666666666666963</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>